<commit_message>
Update Critères de fonctions.xlsx
</commit_message>
<xml_diff>
--- a/PDCA4 (Analyse fonctionnelle)/Critères de fonctions.xlsx
+++ b/PDCA4 (Analyse fonctionnelle)/Critères de fonctions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://viacesifr.sharepoint.com/sites/Groupe_SystmesAutomatises/Documents partages/PDCA4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjetHDD\Ecole\Projet_CESI\2025-2026\Systèmes_automatisés\PDCA4 (Analyse fonctionnelle)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="344" documentId="8_{07749189-F734-48DF-BAED-483BAF4E54D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A90FCC48-3974-43C1-9254-AAD6816CBF13}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C708F4-7C2E-4BC9-81D0-A5A13694F181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{225CFDB5-D927-4728-A221-D9EAC2345C6F}"/>
+    <workbookView xWindow="28680" yWindow="-6390" windowWidth="16440" windowHeight="28590" xr2:uid="{225CFDB5-D927-4728-A221-D9EAC2345C6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -113,9 +113,6 @@
     <t>Fp 2</t>
   </si>
   <si>
-    <t>Alimenter de la colle en mode manuel</t>
-  </si>
-  <si>
     <t>La seringue est remplie sans bulle d’air.</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
   </si>
   <si>
     <t>Fc9/2</t>
-  </si>
-  <si>
-    <t>Fp 3</t>
   </si>
   <si>
     <t>Transférer les capots entre les différentes étapes</t>
@@ -473,6 +467,12 @@
   </si>
   <si>
     <t>0 % d’arrêts non planifiés pour recharger la colle, ou 100 % de disponibilité sur la plage horaire de production.</t>
+  </si>
+  <si>
+    <t>Fc 10</t>
+  </si>
+  <si>
+    <t>Alimentation de la colle</t>
   </si>
 </sst>
 </file>
@@ -955,24 +955,45 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -981,27 +1002,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1021,9 +1021,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1061,7 +1061,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1167,7 +1167,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1309,7 +1309,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1319,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4275FA1D-02FE-4EAD-B9B4-D07D4C2FB99B}">
   <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1332,11 +1332,11 @@
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="17.25">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:22" ht="15.75">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
+      <c r="B1" s="56"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1347,40 +1347,40 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="17.25">
-      <c r="A2" s="58" t="s">
+    <row r="2" spans="1:22">
+      <c r="A2" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="57" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="53" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="17.25">
-      <c r="A3" s="58"/>
-      <c r="B3" s="58"/>
+    <row r="3" spans="1:22">
+      <c r="A3" s="57"/>
+      <c r="B3" s="57"/>
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
     </row>
     <row r="4" spans="1:22" ht="23.25">
-      <c r="A4" s="58"/>
-      <c r="B4" s="58"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="57"/>
       <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="I4" s="30"/>
       <c r="J4" s="31" t="s">
         <v>11</v>
@@ -1422,130 +1422,130 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="32.25">
-      <c r="A5" s="53" t="s">
+    <row r="5" spans="1:22" ht="31.5">
+      <c r="A5" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="54" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="I5" s="31" t="s">
         <v>11</v>
       </c>
       <c r="J5" s="35"/>
       <c r="K5" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="36" t="s">
+      <c r="M5" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="37" t="s">
+      <c r="N5" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="N5" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="O5" s="37" t="s">
+      <c r="P5" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="P5" s="37" t="s">
+      <c r="Q5" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="Q5" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="R5" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="S5" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="T5" s="39" t="s">
+      <c r="U5" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="U5" s="40" t="s">
+      <c r="V5" s="48">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="31.5">
+      <c r="A6" s="54"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="V5" s="60">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="36">
-      <c r="A6" s="53"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="I6" s="31" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="35"/>
       <c r="K6" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="36" t="s">
+      <c r="M6" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="29" t="s">
+      <c r="N6" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="N6" s="37" t="s">
+      <c r="O6" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="37" t="s">
+      <c r="P6" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="R6" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="S6" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q6" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="R6" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="S6" s="38" t="s">
+      <c r="T6" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="T6" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="U6" s="40" t="s">
+      <c r="V6" s="48">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A7" s="54" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="V6" s="60">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A7" s="53" t="s">
+      <c r="C7" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="D7" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="52" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="31" t="s">
@@ -1553,258 +1553,258 @@
       </c>
       <c r="J7" s="35"/>
       <c r="K7" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L7" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M7" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="P7" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q7" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="R7" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="N7" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="O7" s="36" t="s">
+      <c r="S7" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="P7" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q7" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="R7" s="36" t="s">
+      <c r="T7" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="U7" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="S7" s="42" t="s">
+      <c r="V7" s="48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="18.75">
+      <c r="A8" s="54"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="T7" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="U7" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="V7" s="60">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="18.75">
-      <c r="A8" s="53"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
       <c r="I8" s="31" t="s">
         <v>14</v>
       </c>
       <c r="J8" s="35"/>
       <c r="K8" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L8" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M8" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N8" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="O8" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="P8" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="O8" s="37" t="s">
+      <c r="Q8" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="P8" s="37" t="s">
+      <c r="R8" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="Q8" s="37" t="s">
+      <c r="S8" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="R8" s="37" t="s">
+      <c r="T8" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="U8" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="V8" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="18.75">
+      <c r="A9" s="54"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="S8" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="T8" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="U8" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="V8" s="60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="18.75">
-      <c r="A9" s="53"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
       <c r="I9" s="31" t="s">
         <v>15</v>
       </c>
       <c r="J9" s="35"/>
       <c r="K9" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L9" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M9" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N9" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O9" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="P9" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q9" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="R9" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="S9" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="T9" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="U9" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="V9" s="48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="18.75">
+      <c r="A10" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="P9" s="37" t="s">
+      <c r="B10" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="Q9" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="R9" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="S9" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="T9" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="U9" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="V9" s="60">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="18.75">
-      <c r="A10" s="53" t="s">
+      <c r="C10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="D10" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>68</v>
-      </c>
       <c r="E10" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I10" s="31" t="s">
         <v>16</v>
       </c>
       <c r="J10" s="35"/>
       <c r="K10" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L10" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M10" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N10" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O10" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P10" s="37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q10" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="R10" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="S10" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="T10" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="U10" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="V10" s="49">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="30">
+      <c r="A11" s="61"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="R10" s="37" t="s">
+      <c r="D11" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="S10" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="T10" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="U10" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="V10" s="61">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="36">
-      <c r="A11" s="54"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>72</v>
-      </c>
       <c r="E11" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I11" s="31" t="s">
         <v>17</v>
       </c>
       <c r="J11" s="35"/>
       <c r="K11" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L11" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M11" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N11" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O11" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P11" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q11" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="R11" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="S11" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="T11" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="U11" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="V11" s="50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="18.75">
+      <c r="A12" s="62"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="R11" s="37" t="s">
+      <c r="D12" s="12" t="s">
         <v>74</v>
-      </c>
-      <c r="S11" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="T11" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="U11" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="V11" s="62">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="18.75">
-      <c r="A12" s="55"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>76</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>8</v>
@@ -1814,325 +1814,325 @@
       </c>
       <c r="J12" s="35"/>
       <c r="K12" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L12" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M12" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N12" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O12" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P12" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q12" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R12" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="S12" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="T12" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="S12" s="38" t="s">
+      <c r="U12" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="V12" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="23.25" customHeight="1">
+      <c r="A13" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="T12" s="39" t="s">
+      <c r="B13" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="U12" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="V12" s="63">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="23.25" customHeight="1">
-      <c r="A13" s="50" t="s">
+      <c r="C13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="D13" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="E13" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="31" t="s">
         <v>82</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="31" t="s">
-        <v>84</v>
       </c>
       <c r="J13" s="35"/>
       <c r="K13" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L13" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M13" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N13" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O13" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P13" s="35"/>
       <c r="Q13" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R13" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S13" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="T13" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="U13" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="V13" s="48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="18.75">
+      <c r="A14" s="59"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="T13" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="U13" s="40" t="s">
+      <c r="D14" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="V13" s="60">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="18.75">
-      <c r="A14" s="51"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>88</v>
-      </c>
       <c r="E14" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I14" s="31" t="s">
         <v>20</v>
       </c>
       <c r="J14" s="35"/>
       <c r="K14" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L14" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M14" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N14" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O14" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P14" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q14" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R14" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S14" s="46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T14" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U14" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="V14" s="48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="18.75">
+      <c r="A15" s="59"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>89</v>
-      </c>
-      <c r="V14" s="60">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="18.75">
-      <c r="A15" s="51"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>91</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>8</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J15" s="35"/>
       <c r="K15" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L15" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M15" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N15" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O15" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P15" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q15" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R15" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S15" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T15" s="47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U15" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="V15" s="60">
+        <v>44</v>
+      </c>
+      <c r="V15" s="48">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="18.75">
-      <c r="A16" s="52"/>
-      <c r="B16" s="56"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="63"/>
       <c r="C16" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="31" t="s">
         <v>93</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="I16" s="31" t="s">
-        <v>95</v>
       </c>
       <c r="J16" s="35"/>
       <c r="K16" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L16" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M16" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N16" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O16" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P16" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q16" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R16" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S16" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T16" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U16" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="V16" s="60">
+        <v>38</v>
+      </c>
+      <c r="V16" s="48">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="17.25">
+    <row r="17" spans="1:19">
       <c r="A17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="17.25">
+    <row r="18" spans="1:19" ht="15.75">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="E18" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="15.75">
+      <c r="A19" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="B19" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="17.25">
-      <c r="A19" s="3" t="s">
+      <c r="C19" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="D19" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="E19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R19" s="22" t="s">
         <v>105</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="R19" s="22" t="s">
-        <v>107</v>
       </c>
       <c r="S19" s="22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="36">
+    <row r="20" spans="1:19" ht="30">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>110</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>8</v>
@@ -2141,102 +2141,102 @@
         <v>0</v>
       </c>
       <c r="S20" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="30">
+      <c r="A21" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="55" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" ht="36">
-      <c r="A21" s="48" t="s">
+      <c r="C21" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="B21" s="48" t="s">
+      <c r="D21" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="E21" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R21" s="25">
         <v>1</v>
       </c>
       <c r="S21" s="26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="25.5">
+      <c r="A22" s="58"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" ht="27.75">
-      <c r="A22" s="49"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="E22" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R22" s="27">
         <v>2</v>
       </c>
       <c r="S22" s="28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="36" customHeight="1">
+      <c r="A23" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" ht="36" customHeight="1">
-      <c r="A23" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="B23" s="50" t="s">
+      <c r="D23" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>122</v>
       </c>
       <c r="E23" s="8"/>
       <c r="R23" s="25">
         <v>3</v>
       </c>
       <c r="S23" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="15.75">
+      <c r="A24" s="59"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="17.25">
-      <c r="A24" s="51"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>125</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="17.25">
-      <c r="A25" s="51"/>
-      <c r="B25" s="50"/>
+    <row r="25" spans="1:19" ht="15.75">
+      <c r="A25" s="59"/>
+      <c r="B25" s="52"/>
       <c r="C25" s="5"/>
       <c r="D25" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="17.25">
-      <c r="A26" s="52"/>
-      <c r="B26" s="50"/>
+    <row r="26" spans="1:19" ht="15.75">
+      <c r="A26" s="60"/>
+      <c r="B26" s="52"/>
       <c r="C26" s="5"/>
       <c r="D26" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>8</v>
@@ -2247,13 +2247,13 @@
         <v>22</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>130</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>8</v>
@@ -2261,11 +2261,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="A7:A9"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B23:B26"/>
@@ -2280,6 +2275,11 @@
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="B13:B16"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="A7:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2430,12 +2430,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2444,14 +2438,43 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D87B9FBA-51B0-49C9-AB17-4D4ED5C8F1CD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D87B9FBA-51B0-49C9-AB17-4D4ED5C8F1CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="beee2e28-a851-4ac4-9c4a-8792f190b96c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB73F49-B9EF-4C2B-808F-D907317BACCD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2C0FC5A-FC75-42C7-8A5D-1A2D292FF38E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2C0FC5A-FC75-42C7-8A5D-1A2D292FF38E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB73F49-B9EF-4C2B-808F-D907317BACCD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>